<commit_message>
Initial position in collections.xslx
</commit_message>
<xml_diff>
--- a/Presentation/collections.xlsx
+++ b/Presentation/collections.xlsx
@@ -761,8 +761,8 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>